<commit_message>
fixed aggregate discrete range bug
</commit_message>
<xml_diff>
--- a/CDSData/CDSSparse_2020_2021.xlsx
+++ b/CDSData/CDSSparse_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CC6ACF-3D88-47A0-9F72-51AA169F60FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9B80D8-3AD4-48F1-9448-0DDE66AC5E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general info" sheetId="2" r:id="rId1"/>
@@ -270,9 +270,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>The [aggregation] of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [degree-goal] [student_level] students enrolled is &lt;value&gt;</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -1436,6 +1433,9 @@
   </si>
   <si>
     <t>The number of degree-seeking undergraduate (xor [race] {nonresidence alien}) students enrolled is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>The number of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [degree-goal] [student_level] students enrolled is &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -3663,49 +3663,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>27</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3796,7 +3796,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4000,7 +4000,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4068,7 +4068,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4204,7 +4204,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4272,7 +4272,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4408,7 +4408,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4565,52 +4565,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>27</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4704,7 +4704,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4775,7 +4775,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4846,7 +4846,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4917,7 +4917,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4988,7 +4988,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5059,7 +5059,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5201,7 +5201,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5272,7 +5272,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5343,7 +5343,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5414,7 +5414,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5556,7 +5556,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -5627,7 +5627,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5769,7 +5769,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -5929,49 +5929,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>27</v>
@@ -5994,7 +5994,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6062,7 +6062,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6130,7 +6130,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -6198,7 +6198,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6266,7 +6266,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6334,7 +6334,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -6402,7 +6402,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6470,7 +6470,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6538,7 +6538,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -6606,7 +6606,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6674,7 +6674,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -6742,7 +6742,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6810,7 +6810,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -6878,7 +6878,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -6946,7 +6946,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -7014,7 +7014,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -7082,7 +7082,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -7150,7 +7150,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -7218,7 +7218,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -7286,7 +7286,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -7354,7 +7354,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -7422,7 +7422,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -7490,7 +7490,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -7558,7 +7558,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -7626,7 +7626,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -7694,7 +7694,7 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -7762,7 +7762,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -7830,7 +7830,7 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -7898,7 +7898,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -7966,7 +7966,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -8034,7 +8034,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -8102,7 +8102,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -8170,7 +8170,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -8238,7 +8238,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -8306,7 +8306,7 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -8374,7 +8374,7 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -8510,7 +8510,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -8866,67 +8866,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>27</v>
@@ -8949,7 +8949,7 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -9035,7 +9035,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -9121,7 +9121,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -9207,7 +9207,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -9293,7 +9293,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -9379,7 +9379,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -9465,7 +9465,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -9551,7 +9551,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -9637,7 +9637,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -9723,7 +9723,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -9809,7 +9809,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -9981,7 +9981,7 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -10067,7 +10067,7 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -10239,7 +10239,7 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -10427,28 +10427,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>27</v>
@@ -10471,7 +10471,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -10518,7 +10518,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -10565,7 +10565,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -10612,7 +10612,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -10659,7 +10659,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -10706,7 +10706,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -11042,7 +11042,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -11054,91 +11056,91 @@
         <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>9</v>
@@ -11150,10 +11152,10 @@
         <v>24</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>27</v>
@@ -11173,7 +11175,7 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -11298,7 +11300,7 @@
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -11423,7 +11425,7 @@
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -11548,7 +11550,7 @@
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -11673,7 +11675,7 @@
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -11798,7 +11800,7 @@
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -11923,7 +11925,7 @@
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -12048,7 +12050,7 @@
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -12173,7 +12175,7 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -12298,7 +12300,7 @@
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -12423,7 +12425,7 @@
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -12548,7 +12550,7 @@
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -12673,7 +12675,7 @@
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -12798,7 +12800,7 @@
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -12923,7 +12925,7 @@
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -13048,7 +13050,7 @@
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -13173,7 +13175,7 @@
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -13298,7 +13300,7 @@
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -13423,7 +13425,7 @@
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -13548,7 +13550,7 @@
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -13673,7 +13675,7 @@
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -14439,16 +14441,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>47</v>
@@ -14477,7 +14479,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -14518,7 +14520,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -14600,7 +14602,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -14641,7 +14643,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -14764,7 +14766,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -14805,7 +14807,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -14846,7 +14848,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -14985,10 +14987,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>27</v>
@@ -15008,7 +15010,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -15034,7 +15036,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -15206,7 +15208,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>49</v>
@@ -15224,46 +15226,46 @@
         <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>361</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>27</v>
@@ -15283,7 +15285,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15363,7 +15365,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -15443,7 +15445,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -15523,7 +15525,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -15603,7 +15605,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -15683,7 +15685,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -15763,7 +15765,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -15843,7 +15845,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -15923,7 +15925,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -16003,7 +16005,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -16083,7 +16085,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -16163,7 +16165,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -16243,7 +16245,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -16323,7 +16325,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -16403,7 +16405,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -16483,7 +16485,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -16979,37 +16981,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>27</v>
@@ -17029,7 +17031,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -17082,7 +17084,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -17135,7 +17137,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -17188,7 +17190,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -17241,7 +17243,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -17566,9 +17568,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A11" sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="114.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -19612,7 +19619,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>462</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -19680,7 +19687,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -19748,7 +19755,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -19816,7 +19823,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -19952,6 +19959,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -19959,76 +19967,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="9" max="9" width="21.21875" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>393</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>401</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>27</v>
@@ -20048,7 +20064,7 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -20131,7 +20147,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -20214,7 +20230,7 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -20297,7 +20313,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -20380,7 +20396,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -20463,7 +20479,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -20546,7 +20562,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -20629,7 +20645,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -20712,7 +20728,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -20795,7 +20811,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -20878,7 +20894,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -20961,7 +20977,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -21044,7 +21060,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -21127,7 +21143,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -21210,7 +21226,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -21293,7 +21309,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -21376,7 +21392,7 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -21459,7 +21475,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -21542,7 +21558,7 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -22040,7 +22056,7 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -22123,7 +22139,7 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -22388,13 +22404,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>49</v>
@@ -22406,64 +22422,64 @@
         <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>424</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>27</v>
@@ -22483,7 +22499,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -22581,7 +22597,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -22679,7 +22695,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -22777,7 +22793,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -22875,7 +22891,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -22973,7 +22989,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -23071,7 +23087,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -23169,7 +23185,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -23267,7 +23283,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -23365,7 +23381,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -23463,7 +23479,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -23561,7 +23577,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -23659,7 +23675,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -23757,7 +23773,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -24149,7 +24165,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -24247,7 +24263,7 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -24557,13 +24573,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>48</v>
@@ -24575,63 +24591,63 @@
         <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -24708,7 +24724,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -24785,7 +24801,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -24862,7 +24878,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -24939,7 +24955,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -25016,7 +25032,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -25093,7 +25109,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -25170,7 +25186,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -25247,7 +25263,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -25324,7 +25340,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -25401,7 +25417,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -25478,7 +25494,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -25555,7 +25571,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -25632,7 +25648,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -25879,13 +25895,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>48</v>
@@ -25897,58 +25913,58 @@
         <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
@@ -26492,7 +26508,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -26569,7 +26585,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -26646,7 +26662,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -26723,7 +26739,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -26800,7 +26816,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -26877,7 +26893,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -26954,7 +26970,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -27204,7 +27220,7 @@
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>54</v>
@@ -27317,25 +27333,25 @@
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>458</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -27594,19 +27610,19 @@
         <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -27696,8 +27712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27719,40 +27735,40 @@
         <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>67</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>27</v>
@@ -27773,12 +27789,12 @@
         <v>31</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -27849,7 +27865,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -27920,7 +27936,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -27991,7 +28007,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -28133,7 +28149,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -28275,7 +28291,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -28346,7 +28362,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -28488,7 +28504,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -28843,7 +28859,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -28921,9 +28937,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="94.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -28942,40 +28963,40 @@
         <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>67</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>27</v>
@@ -28996,12 +29017,12 @@
         <v>31</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -29075,7 +29096,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -29149,7 +29170,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -29223,7 +29244,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -29371,7 +29392,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -29519,7 +29540,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -29741,7 +29762,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -30111,7 +30132,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -30192,88 +30213,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>72</v>
@@ -30299,7 +30356,7 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -30400,7 +30457,7 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -30501,7 +30558,7 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -30905,7 +30962,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -31006,7 +31063,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -31107,7 +31164,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -31208,7 +31265,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -31309,7 +31366,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -31410,7 +31467,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -31511,7 +31568,7 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -31713,7 +31770,7 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -32117,7 +32174,7 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -32218,7 +32275,7 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -32319,7 +32376,7 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -32420,7 +32477,7 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -32521,7 +32578,7 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -32622,7 +32679,7 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -32723,6 +32780,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -32739,70 +32797,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>27</v>
@@ -32813,7 +32871,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -32890,7 +32948,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -32967,7 +33025,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -33044,7 +33102,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -33121,7 +33179,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -33198,7 +33256,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -33275,7 +33333,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -33352,7 +33410,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -33429,7 +33487,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -33506,7 +33564,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -33583,7 +33641,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -33660,7 +33718,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -33737,7 +33795,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -33814,7 +33872,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -33891,7 +33949,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -33968,7 +34026,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -34045,7 +34103,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -34122,7 +34180,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -34199,7 +34257,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -34276,7 +34334,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -34353,7 +34411,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -34446,67 +34504,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>27</v>
@@ -34514,7 +34572,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -34585,7 +34643,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -34656,7 +34714,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -34727,7 +34785,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -34798,7 +34856,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -34869,7 +34927,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -34940,7 +34998,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -35011,7 +35069,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -35082,7 +35140,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -35153,7 +35211,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -35224,7 +35282,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -35384,52 +35442,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>27</v>
@@ -35452,7 +35510,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -35523,7 +35581,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -35594,7 +35652,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -35665,7 +35723,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -35736,7 +35794,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -35807,7 +35865,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -35949,7 +36007,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -36020,7 +36078,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -36162,7 +36220,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -36312,7 +36370,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36326,58 +36384,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>27</v>
@@ -36400,7 +36458,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -36477,7 +36535,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -36554,7 +36612,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -36631,7 +36689,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -36708,7 +36766,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -36785,7 +36843,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -36862,7 +36920,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -36939,7 +36997,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -37016,7 +37074,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -37093,7 +37151,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -37170,7 +37228,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -37247,7 +37305,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -37401,7 +37459,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -37478,7 +37536,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -37632,7 +37690,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18">
         <v>0</v>

</xml_diff>